<commit_message>
Footer and Bodies for Home, AboutUs and Ship
</commit_message>
<xml_diff>
--- a/listOfComponentsToMake.xlsx
+++ b/listOfComponentsToMake.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkaln\Desktop\NuCamp\3-React\projecttomato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E2872-B69F-462E-BC08-14D6DE7220B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B71890B-A376-4143-9D6A-51EE45BAE253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04E0F70B-8672-475B-BEB4-2105540DEA69}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Tomato Components Matchup</t>
   </si>
@@ -48,33 +48,15 @@
     <t>Index.html</t>
   </si>
   <si>
-    <t>img</t>
-  </si>
-  <si>
-    <t>HomeSalesCopyComponent.js</t>
-  </si>
-  <si>
     <t>LinksComponent.js</t>
   </si>
   <si>
-    <t>ContactUsInfoComponent.js</t>
-  </si>
-  <si>
-    <t>ContactFormComponent.js</t>
-  </si>
-  <si>
-    <t>LogoComponent.js</t>
-  </si>
-  <si>
     <t>HeaderComponent.js</t>
   </si>
   <si>
     <t>MainComponent.js</t>
   </si>
   <si>
-    <t>HomeComponent.js</t>
-  </si>
-  <si>
     <t>AboutUsComponent.js</t>
   </si>
   <si>
@@ -93,12 +75,6 @@
     <t>Styles.css</t>
   </si>
   <si>
-    <t>AboutUsSalesCopyComponent.js</t>
-  </si>
-  <si>
-    <t>ShipSalesCopyComponent.js</t>
-  </si>
-  <si>
     <t>App.js</t>
   </si>
   <si>
@@ -121,13 +97,49 @@
   </si>
   <si>
     <t>FooterComponent.js</t>
+  </si>
+  <si>
+    <t>SocialLinksComponent.js</t>
+  </si>
+  <si>
+    <t>NBarLinks</t>
+  </si>
+  <si>
+    <t>NBarSocialLinks</t>
+  </si>
+  <si>
+    <t>Nbar</t>
+  </si>
+  <si>
+    <t>HomeComp</t>
+  </si>
+  <si>
+    <t>HomeComp.js</t>
+  </si>
+  <si>
+    <t>public/assets/images</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>AboutUs</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that the className "foodPic"'s are added for foodpicture backgrounds to be done in CSS, and  Note that the className "getFrosty" is added for frosted glass in CSS. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +147,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,8 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,162 +501,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78A570A-DB53-4E2F-8B2E-18DF8847644F}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="C29" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>